<commit_message>
review the code Gabriel-Greg
</commit_message>
<xml_diff>
--- a/BddGreg/automation.xlsx
+++ b/BddGreg/automation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtranulo\eclipse-workspace\CucumberTestAutomation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gbujnows\Desktop\BDDDataDriven\BddGreg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C69890-FBBE-4358-8D4D-82E4C2E737C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E07AB6-F158-4AF7-99DF-CCF286022904}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2830" yWindow="1300" windowWidth="14400" windowHeight="7460" xr2:uid="{D49A02D6-1CAD-4228-9FE1-F8829C14B003}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D49A02D6-1CAD-4228-9FE1-F8829C14B003}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>Roman</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -400,56 +409,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F1D22C-B9F1-4879-A2E3-4621C1D4117A}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6328125" customWidth="1"/>
+    <col min="2" max="2" width="23.6328125" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>12345</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>12345</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>12345</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>12345</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Clean Version ready to use
</commit_message>
<xml_diff>
--- a/BddGreg/automation.xlsx
+++ b/BddGreg/automation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gbujnows\Desktop\BDDDataDriven\BddGreg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E07AB6-F158-4AF7-99DF-CCF286022904}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE69E209-FA5A-41BC-BFE5-6146D710574A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D49A02D6-1CAD-4228-9FE1-F8829C14B003}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
 </sst>
 </file>
@@ -411,7 +408,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F1D22C-B9F1-4879-A2E3-4621C1D4117A}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -457,7 +456,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -468,7 +467,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -484,6 +483,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E96B55406D4C8E48A9AAAB23DAEFCC43" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c6c6032683a10b9c07cac5cc62f3c848">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fad91024-48b7-4fce-a49d-d3458c86d56c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d5c9ef1d4e60b8573d4781a27392ff3e" ns2:_="">
     <xsd:import namespace="fad91024-48b7-4fce-a49d-d3458c86d56c"/>
@@ -629,22 +643,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD865F64-A5E4-4C29-ABDA-21288892AFB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49A84303-2422-4452-B562-DD28EB8DD2B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{504FF294-051A-4DED-A269-FE4529791CF5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -660,21 +676,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49A84303-2422-4452-B562-DD28EB8DD2B7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD865F64-A5E4-4C29-ABDA-21288892AFB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>